<commit_message>
changed to Future / cleaned Repos
</commit_message>
<xml_diff>
--- a/server/conf/excel/excel.xlsx
+++ b/server/conf/excel/excel.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpa/dev/Github/experiments/play-binding-petstore/server/conf/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D46242-6065-514E-86DF-009E27D2AC51}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCE5AE3-79C5-A448-A37F-79058D08551C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4240" yWindow="460" windowWidth="29360" windowHeight="12780" tabRatio="934" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="16" r:id="rId1"/>
     <sheet name="products" sheetId="2" r:id="rId2"/>
     <sheet name="pets" sheetId="3" r:id="rId3"/>
+    <sheet name="users" sheetId="17" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -411,6 +412,87 @@
   </si>
   <si>
     <t>HAM-0001</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Groupds</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>demoCustomer</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Caprio</t>
+  </si>
+  <si>
+    <t>peter@caprio.com</t>
+  </si>
+  <si>
+    <t>caprio.jpg</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>demoManager</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Reeves</t>
+  </si>
+  <si>
+    <t>kent@petstore.com</t>
+  </si>
+  <si>
+    <t>reeves.jpg</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>demoAdmin</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Devito</t>
+  </si>
+  <si>
+    <t>daniel@petstore.com</t>
+  </si>
+  <si>
+    <t>devito.jpg</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -789,7 +871,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="183" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -874,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="160" workbookViewId="0">
+    <sheetView zoomScale="160" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -1118,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="225" workbookViewId="0">
+    <sheetView zoomScale="225" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -1702,4 +1784,118 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB2D3C8-E974-204A-9043-47C23044568C}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>